<commit_message>
Typos corrected in calibration procedure
</commit_message>
<xml_diff>
--- a/ETC v2/v2.2/DStage_ETC_v2.2_calibration.xlsx
+++ b/ETC v2/v2.2/DStage_ETC_v2.2_calibration.xlsx
@@ -136,7 +136,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t>input. Put the measured vakue into the field below.</t>
+      <t>input. Put the measured value into the field below.</t>
     </r>
   </si>
   <si>
@@ -196,17 +196,24 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>Step 4</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> - Keep the throttle oppened manually and measure the voltage at TH input. Put the measured vakue into the field below.</t>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Step 4 - Keep the gas pedal fully pressed and measure the voltage at </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">GP </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t>input. Put the measured value into the field below.</t>
     </r>
   </si>
   <si>
@@ -407,7 +414,7 @@
     <t>required gain for gas pedal input</t>
   </si>
   <si>
-    <t>required offset gas pedal input</t>
+    <t>required offset for gas pedal input</t>
   </si>
   <si>
     <t>Step 8</t>

</xml_diff>